<commit_message>
Update view of sheet
</commit_message>
<xml_diff>
--- a/Input/Tier_Classification_of_SDG_Indicators_29_Mar_2021_web.xlsx
+++ b/Input/Tier_Classification_of_SDG_Indicators_29_Mar_2021_web.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\sdg_tier_classifications\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B420E03-7DC3-40E6-877A-BDC3F401331B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0167145-F76B-419B-97CB-84765DF30498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="1" r:id="rId1"/>
@@ -6190,18 +6190,6 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -6228,6 +6216,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="73">
@@ -6686,15 +6686,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27.6" x14ac:dyDescent="0.45">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
     </row>
     <row r="2" spans="1:18" s="10" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -6726,15 +6726,15 @@
       <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:18" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="83"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="92"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
@@ -7132,25 +7132,25 @@
       <c r="N16" s="22"/>
     </row>
     <row r="17" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="83" t="s">
+      <c r="C17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I17" s="14"/>
@@ -7576,25 +7576,25 @@
       <c r="N31" s="22"/>
     </row>
     <row r="32" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="81" t="s">
+      <c r="B32" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="83" t="s">
+      <c r="C32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I32" s="14"/>
@@ -8438,25 +8438,25 @@
       <c r="N60" s="22"/>
     </row>
     <row r="61" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="81" t="s">
+      <c r="B61" s="90" t="s">
         <v>220</v>
       </c>
-      <c r="C61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="83" t="s">
+      <c r="C61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I61" s="14"/>
@@ -8824,25 +8824,25 @@
       <c r="N73" s="22"/>
     </row>
     <row r="74" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="81" t="s">
+      <c r="B74" s="90" t="s">
         <v>273</v>
       </c>
-      <c r="C74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H74" s="83" t="s">
+      <c r="C74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H74" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I74" s="14"/>
@@ -9270,25 +9270,25 @@
       <c r="N88" s="22"/>
     </row>
     <row r="89" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="81" t="s">
+      <c r="B89" s="90" t="s">
         <v>333</v>
       </c>
-      <c r="C89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H89" s="83" t="s">
+      <c r="C89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H89" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I89" s="14"/>
@@ -9626,25 +9626,25 @@
       <c r="N100" s="22"/>
     </row>
     <row r="101" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="81" t="s">
+      <c r="B101" s="90" t="s">
         <v>382</v>
       </c>
-      <c r="C101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H101" s="83" t="s">
+      <c r="C101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H101" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I101" s="14"/>
@@ -9830,25 +9830,25 @@
       <c r="N107" s="22"/>
     </row>
     <row r="108" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="81" t="s">
+      <c r="B108" s="90" t="s">
         <v>410</v>
       </c>
-      <c r="C108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H108" s="83" t="s">
+      <c r="C108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H108" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I108" s="14"/>
@@ -10336,25 +10336,25 @@
       <c r="N124" s="22"/>
     </row>
     <row r="125" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="81" t="s">
+      <c r="B125" s="90" t="s">
         <v>469</v>
       </c>
-      <c r="C125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H125" s="83" t="s">
+      <c r="C125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H125" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I125" s="14"/>
@@ -10722,25 +10722,25 @@
       <c r="N137" s="22"/>
     </row>
     <row r="138" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="81" t="s">
+      <c r="B138" s="90" t="s">
         <v>511</v>
       </c>
-      <c r="C138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H138" s="83" t="s">
+      <c r="C138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H138" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I138" s="14"/>
@@ -11158,25 +11158,25 @@
       <c r="N152" s="22"/>
     </row>
     <row r="153" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="81" t="s">
+      <c r="B153" s="90" t="s">
         <v>571</v>
       </c>
-      <c r="C153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H153" s="83" t="s">
+      <c r="C153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H153" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I153" s="14"/>
@@ -11619,25 +11619,25 @@
       <c r="N168" s="22"/>
     </row>
     <row r="169" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="81" t="s">
+      <c r="B169" s="90" t="s">
         <v>620</v>
       </c>
-      <c r="C169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H169" s="83" t="s">
+      <c r="C169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H169" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I169" s="14"/>
@@ -12031,25 +12031,25 @@
       <c r="N182" s="22"/>
     </row>
     <row r="183" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="81" t="s">
+      <c r="B183" s="90" t="s">
         <v>667</v>
       </c>
-      <c r="C183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H183" s="83" t="s">
+      <c r="C183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H183" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I183" s="14"/>
@@ -12285,25 +12285,25 @@
       <c r="N191" s="22"/>
     </row>
     <row r="192" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="81" t="s">
+      <c r="B192" s="90" t="s">
         <v>691</v>
       </c>
-      <c r="C192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H192" s="83" t="s">
+      <c r="C192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H192" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I192" s="14"/>
@@ -12613,25 +12613,25 @@
       <c r="N202" s="22"/>
     </row>
     <row r="203" spans="1:14" s="13" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="81" t="s">
+      <c r="B203" s="90" t="s">
         <v>735</v>
       </c>
-      <c r="C203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H203" s="83" t="s">
+      <c r="C203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H203" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I203" s="14"/>
@@ -13059,25 +13059,25 @@
       <c r="N217" s="22"/>
     </row>
     <row r="218" spans="1:14" s="13" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B218" s="81" t="s">
+      <c r="B218" s="90" t="s">
         <v>792</v>
       </c>
-      <c r="C218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H218" s="83" t="s">
+      <c r="C218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H218" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I218" s="14"/>
@@ -13803,25 +13803,25 @@
       <c r="N242" s="22"/>
     </row>
     <row r="243" spans="1:14" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B243" s="81" t="s">
+      <c r="B243" s="90" t="s">
         <v>879</v>
       </c>
-      <c r="C243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H243" s="83" t="s">
+      <c r="C243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H243" s="92" t="s">
         <v>22</v>
       </c>
       <c r="I243" s="14"/>
@@ -13829,15 +13829,15 @@
       <c r="K243" s="14"/>
     </row>
     <row r="244" spans="1:14" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B244" s="86" t="s">
+      <c r="B244" s="82" t="s">
         <v>880</v>
       </c>
-      <c r="C244" s="87"/>
-      <c r="D244" s="87"/>
-      <c r="E244" s="87"/>
-      <c r="F244" s="87"/>
-      <c r="G244" s="87"/>
-      <c r="H244" s="88"/>
+      <c r="C244" s="83"/>
+      <c r="D244" s="83"/>
+      <c r="E244" s="83"/>
+      <c r="F244" s="83"/>
+      <c r="G244" s="83"/>
+      <c r="H244" s="84"/>
       <c r="I244" s="22"/>
       <c r="J244" s="22"/>
       <c r="K244" s="22"/>
@@ -14056,15 +14056,15 @@
       <c r="N251" s="22"/>
     </row>
     <row r="252" spans="1:14" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B252" s="86" t="s">
+      <c r="B252" s="82" t="s">
         <v>907</v>
       </c>
-      <c r="C252" s="87"/>
-      <c r="D252" s="87"/>
-      <c r="E252" s="87"/>
-      <c r="F252" s="87"/>
-      <c r="G252" s="87"/>
-      <c r="H252" s="88"/>
+      <c r="C252" s="83"/>
+      <c r="D252" s="83"/>
+      <c r="E252" s="83"/>
+      <c r="F252" s="83"/>
+      <c r="G252" s="83"/>
+      <c r="H252" s="84"/>
       <c r="I252" s="22"/>
       <c r="J252" s="22"/>
       <c r="K252" s="22"/>
@@ -14161,15 +14161,15 @@
       <c r="N255" s="22"/>
     </row>
     <row r="256" spans="1:14" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B256" s="86" t="s">
+      <c r="B256" s="82" t="s">
         <v>919</v>
       </c>
-      <c r="C256" s="87"/>
-      <c r="D256" s="87"/>
-      <c r="E256" s="87"/>
-      <c r="F256" s="87"/>
-      <c r="G256" s="87"/>
-      <c r="H256" s="88"/>
+      <c r="C256" s="83"/>
+      <c r="D256" s="83"/>
+      <c r="E256" s="83"/>
+      <c r="F256" s="83"/>
+      <c r="G256" s="83"/>
+      <c r="H256" s="84"/>
       <c r="I256" s="22"/>
       <c r="J256" s="22"/>
       <c r="K256" s="22"/>
@@ -14206,15 +14206,15 @@
       <c r="N257" s="22"/>
     </row>
     <row r="258" spans="1:14" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B258" s="86" t="s">
+      <c r="B258" s="82" t="s">
         <v>923</v>
       </c>
-      <c r="C258" s="87"/>
-      <c r="D258" s="87"/>
-      <c r="E258" s="87"/>
-      <c r="F258" s="87"/>
-      <c r="G258" s="87"/>
-      <c r="H258" s="88"/>
+      <c r="C258" s="83"/>
+      <c r="D258" s="83"/>
+      <c r="E258" s="83"/>
+      <c r="F258" s="83"/>
+      <c r="G258" s="83"/>
+      <c r="H258" s="84"/>
       <c r="I258" s="22"/>
       <c r="J258" s="22"/>
       <c r="K258" s="22"/>
@@ -14311,30 +14311,30 @@
       <c r="N261" s="22"/>
     </row>
     <row r="262" spans="1:14" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B262" s="86" t="s">
+      <c r="B262" s="82" t="s">
         <v>934</v>
       </c>
-      <c r="C262" s="87"/>
-      <c r="D262" s="87"/>
-      <c r="E262" s="87"/>
-      <c r="F262" s="87"/>
-      <c r="G262" s="87"/>
-      <c r="H262" s="88"/>
+      <c r="C262" s="83"/>
+      <c r="D262" s="83"/>
+      <c r="E262" s="83"/>
+      <c r="F262" s="83"/>
+      <c r="G262" s="83"/>
+      <c r="H262" s="84"/>
       <c r="I262" s="22"/>
       <c r="J262" s="22"/>
       <c r="K262" s="22"/>
       <c r="N262" s="22"/>
     </row>
     <row r="263" spans="1:14" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B263" s="89" t="s">
+      <c r="B263" s="85" t="s">
         <v>935</v>
       </c>
-      <c r="C263" s="90"/>
-      <c r="D263" s="90"/>
-      <c r="E263" s="90"/>
-      <c r="F263" s="90"/>
-      <c r="G263" s="90"/>
-      <c r="H263" s="91"/>
+      <c r="C263" s="86"/>
+      <c r="D263" s="86"/>
+      <c r="E263" s="86"/>
+      <c r="F263" s="86"/>
+      <c r="G263" s="86"/>
+      <c r="H263" s="87"/>
       <c r="I263" s="22"/>
       <c r="J263" s="22"/>
       <c r="K263" s="22"/>
@@ -14431,15 +14431,15 @@
       <c r="N266" s="22"/>
     </row>
     <row r="267" spans="1:14" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B267" s="89" t="s">
+      <c r="B267" s="85" t="s">
         <v>947</v>
       </c>
-      <c r="C267" s="90"/>
-      <c r="D267" s="90"/>
-      <c r="E267" s="90"/>
-      <c r="F267" s="90"/>
-      <c r="G267" s="90"/>
-      <c r="H267" s="91"/>
+      <c r="C267" s="86"/>
+      <c r="D267" s="86"/>
+      <c r="E267" s="86"/>
+      <c r="F267" s="86"/>
+      <c r="G267" s="86"/>
+      <c r="H267" s="87"/>
       <c r="I267" s="22"/>
       <c r="J267" s="22"/>
       <c r="K267" s="22"/>
@@ -14504,15 +14504,15 @@
       <c r="N269" s="22"/>
     </row>
     <row r="270" spans="1:14" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B270" s="89" t="s">
+      <c r="B270" s="85" t="s">
         <v>955</v>
       </c>
-      <c r="C270" s="90"/>
-      <c r="D270" s="90"/>
-      <c r="E270" s="90"/>
-      <c r="F270" s="90"/>
-      <c r="G270" s="90"/>
-      <c r="H270" s="91"/>
+      <c r="C270" s="86"/>
+      <c r="D270" s="86"/>
+      <c r="E270" s="86"/>
+      <c r="F270" s="86"/>
+      <c r="G270" s="86"/>
+      <c r="H270" s="87"/>
       <c r="I270" s="22"/>
       <c r="J270" s="22"/>
       <c r="K270" s="22"/>
@@ -14663,57 +14663,57 @@
       <c r="N275" s="22"/>
     </row>
     <row r="276" spans="1:14" s="57" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B276" s="92" t="s">
+      <c r="B276" s="88" t="s">
         <v>972</v>
       </c>
-      <c r="C276" s="92"/>
-      <c r="D276" s="92"/>
-      <c r="E276" s="92"/>
-      <c r="F276" s="92"/>
-      <c r="G276" s="92"/>
-      <c r="H276" s="92"/>
+      <c r="C276" s="88"/>
+      <c r="D276" s="88"/>
+      <c r="E276" s="88"/>
+      <c r="F276" s="88"/>
+      <c r="G276" s="88"/>
+      <c r="H276" s="88"/>
       <c r="I276" s="56"/>
       <c r="J276" s="56"/>
       <c r="K276" s="56"/>
     </row>
     <row r="277" spans="1:14" s="57" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B277" s="93" t="s">
+      <c r="B277" s="89" t="s">
         <v>973</v>
       </c>
-      <c r="C277" s="93"/>
-      <c r="D277" s="93"/>
-      <c r="E277" s="93"/>
-      <c r="F277" s="93"/>
-      <c r="G277" s="93"/>
-      <c r="H277" s="93"/>
+      <c r="C277" s="89"/>
+      <c r="D277" s="89"/>
+      <c r="E277" s="89"/>
+      <c r="F277" s="89"/>
+      <c r="G277" s="89"/>
+      <c r="H277" s="89"/>
       <c r="I277" s="56"/>
       <c r="J277" s="56"/>
       <c r="K277" s="56"/>
     </row>
     <row r="278" spans="1:14" s="57" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B278" s="93" t="s">
+      <c r="B278" s="89" t="s">
         <v>974</v>
       </c>
-      <c r="C278" s="93"/>
-      <c r="D278" s="93"/>
-      <c r="E278" s="93"/>
-      <c r="F278" s="93"/>
-      <c r="G278" s="93"/>
-      <c r="H278" s="93"/>
+      <c r="C278" s="89"/>
+      <c r="D278" s="89"/>
+      <c r="E278" s="89"/>
+      <c r="F278" s="89"/>
+      <c r="G278" s="89"/>
+      <c r="H278" s="89"/>
       <c r="I278" s="56"/>
       <c r="J278" s="56"/>
       <c r="K278" s="56"/>
     </row>
     <row r="279" spans="1:14" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B279" s="85" t="s">
+      <c r="B279" s="81" t="s">
         <v>975</v>
       </c>
-      <c r="C279" s="85"/>
-      <c r="D279" s="85"/>
-      <c r="E279" s="85"/>
-      <c r="F279" s="85"/>
-      <c r="G279" s="85"/>
-      <c r="H279" s="85"/>
+      <c r="C279" s="81"/>
+      <c r="D279" s="81"/>
+      <c r="E279" s="81"/>
+      <c r="F279" s="81"/>
+      <c r="G279" s="81"/>
+      <c r="H279" s="81"/>
       <c r="I279" s="56"/>
       <c r="J279" s="56"/>
       <c r="K279" s="56"/>
@@ -14721,6 +14721,24 @@
   </sheetData>
   <autoFilter ref="A2:I279" xr:uid="{6B1B4B68-CDE7-4773-B6E3-1B4E74E676EC}"/>
   <mergeCells count="30">
+    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B243:H243"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="B101:H101"/>
+    <mergeCell ref="B108:H108"/>
+    <mergeCell ref="B125:H125"/>
+    <mergeCell ref="B138:H138"/>
+    <mergeCell ref="B153:H153"/>
+    <mergeCell ref="B169:H169"/>
+    <mergeCell ref="B183:H183"/>
+    <mergeCell ref="B192:H192"/>
+    <mergeCell ref="B203:H203"/>
+    <mergeCell ref="B218:H218"/>
     <mergeCell ref="B279:H279"/>
     <mergeCell ref="B244:H244"/>
     <mergeCell ref="B252:H252"/>
@@ -14733,24 +14751,6 @@
     <mergeCell ref="B276:H276"/>
     <mergeCell ref="B277:H277"/>
     <mergeCell ref="B278:H278"/>
-    <mergeCell ref="B243:H243"/>
-    <mergeCell ref="B89:H89"/>
-    <mergeCell ref="B101:H101"/>
-    <mergeCell ref="B108:H108"/>
-    <mergeCell ref="B125:H125"/>
-    <mergeCell ref="B138:H138"/>
-    <mergeCell ref="B153:H153"/>
-    <mergeCell ref="B169:H169"/>
-    <mergeCell ref="B183:H183"/>
-    <mergeCell ref="B192:H192"/>
-    <mergeCell ref="B203:H203"/>
-    <mergeCell ref="B218:H218"/>
-    <mergeCell ref="B74:H74"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B61:H61"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
   <pageSetup scale="84" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -14941,8 +14941,8 @@
   </sheetPr>
   <dimension ref="A1:I279"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14960,15 +14960,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.45">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="93" t="s">
         <v>1079</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
       <c r="I1" s="73"/>
     </row>
     <row r="2" spans="1:9" s="77" customFormat="1" ht="50.4" x14ac:dyDescent="0.3">
@@ -15001,15 +15001,15 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="83"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="92"/>
     </row>
     <row r="4" spans="1:9" s="71" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
@@ -15365,25 +15365,25 @@
       <c r="I16" s="74"/>
     </row>
     <row r="17" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="83" t="s">
+      <c r="C17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -15776,25 +15776,25 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="81" t="s">
+      <c r="B32" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="83" t="s">
+      <c r="C32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -16575,25 +16575,25 @@
       <c r="I60" s="74"/>
     </row>
     <row r="61" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="81" t="s">
+      <c r="B61" s="90" t="s">
         <v>220</v>
       </c>
-      <c r="C61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G61" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="83" t="s">
+      <c r="C61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -16934,25 +16934,25 @@
       </c>
     </row>
     <row r="74" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="81" t="s">
+      <c r="B74" s="90" t="s">
         <v>273</v>
       </c>
-      <c r="C74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G74" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H74" s="83" t="s">
+      <c r="C74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H74" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -17345,25 +17345,25 @@
       </c>
     </row>
     <row r="89" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="81" t="s">
+      <c r="B89" s="90" t="s">
         <v>333</v>
       </c>
-      <c r="C89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G89" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H89" s="83" t="s">
+      <c r="C89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G89" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H89" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -17673,25 +17673,25 @@
       </c>
     </row>
     <row r="101" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="81" t="s">
+      <c r="B101" s="90" t="s">
         <v>382</v>
       </c>
-      <c r="C101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G101" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H101" s="83" t="s">
+      <c r="C101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G101" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H101" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -17866,25 +17866,25 @@
       </c>
     </row>
     <row r="108" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="81" t="s">
+      <c r="B108" s="90" t="s">
         <v>410</v>
       </c>
-      <c r="C108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G108" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H108" s="83" t="s">
+      <c r="C108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G108" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H108" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -18341,25 +18341,25 @@
       </c>
     </row>
     <row r="125" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="81" t="s">
+      <c r="B125" s="90" t="s">
         <v>469</v>
       </c>
-      <c r="C125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G125" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H125" s="83" t="s">
+      <c r="C125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G125" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H125" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -18704,25 +18704,25 @@
       </c>
     </row>
     <row r="138" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="81" t="s">
+      <c r="B138" s="90" t="s">
         <v>511</v>
       </c>
-      <c r="C138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G138" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H138" s="83" t="s">
+      <c r="C138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G138" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H138" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -19095,25 +19095,25 @@
       </c>
     </row>
     <row r="153" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="81" t="s">
+      <c r="B153" s="90" t="s">
         <v>571</v>
       </c>
-      <c r="C153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G153" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H153" s="83" t="s">
+      <c r="C153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G153" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H153" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -19526,25 +19526,25 @@
       <c r="I168" s="74"/>
     </row>
     <row r="169" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="81" t="s">
+      <c r="B169" s="90" t="s">
         <v>620</v>
       </c>
-      <c r="C169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G169" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H169" s="83" t="s">
+      <c r="C169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G169" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H169" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -19910,25 +19910,25 @@
       </c>
     </row>
     <row r="183" spans="1:9" s="70" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="81" t="s">
+      <c r="B183" s="90" t="s">
         <v>667</v>
       </c>
-      <c r="C183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G183" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H183" s="83" t="s">
+      <c r="C183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G183" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H183" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -20143,25 +20143,25 @@
       </c>
     </row>
     <row r="192" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="81" t="s">
+      <c r="B192" s="90" t="s">
         <v>691</v>
       </c>
-      <c r="C192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G192" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H192" s="83" t="s">
+      <c r="C192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G192" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H192" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -20444,25 +20444,25 @@
       </c>
     </row>
     <row r="203" spans="1:9" s="70" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="81" t="s">
+      <c r="B203" s="90" t="s">
         <v>735</v>
       </c>
-      <c r="C203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G203" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H203" s="83" t="s">
+      <c r="C203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G203" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H203" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -20857,25 +20857,25 @@
       </c>
     </row>
     <row r="218" spans="1:9" s="70" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B218" s="81" t="s">
+      <c r="B218" s="90" t="s">
         <v>792</v>
       </c>
-      <c r="C218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G218" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H218" s="83" t="s">
+      <c r="C218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G218" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H218" s="92" t="s">
         <v>22</v>
       </c>
     </row>
@@ -21544,38 +21544,38 @@
       </c>
     </row>
     <row r="243" spans="1:9" s="70" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B243" s="81" t="s">
+      <c r="B243" s="90" t="s">
         <v>879</v>
       </c>
-      <c r="C243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="F243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="G243" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="H243" s="83" t="s">
+      <c r="C243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="F243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="G243" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H243" s="92" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="244" spans="1:9" s="71" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B244" s="86" t="s">
+      <c r="B244" s="82" t="s">
         <v>880</v>
       </c>
-      <c r="C244" s="87"/>
-      <c r="D244" s="87"/>
-      <c r="E244" s="87"/>
-      <c r="F244" s="87"/>
-      <c r="G244" s="87"/>
-      <c r="H244" s="88"/>
+      <c r="C244" s="83"/>
+      <c r="D244" s="83"/>
+      <c r="E244" s="83"/>
+      <c r="F244" s="83"/>
+      <c r="G244" s="83"/>
+      <c r="H244" s="84"/>
     </row>
     <row r="245" spans="1:9" s="71" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="71" t="s">
@@ -21779,15 +21779,15 @@
       </c>
     </row>
     <row r="252" spans="1:9" s="71" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B252" s="86" t="s">
+      <c r="B252" s="82" t="s">
         <v>907</v>
       </c>
-      <c r="C252" s="87"/>
-      <c r="D252" s="87"/>
-      <c r="E252" s="87"/>
-      <c r="F252" s="87"/>
-      <c r="G252" s="87"/>
-      <c r="H252" s="88"/>
+      <c r="C252" s="83"/>
+      <c r="D252" s="83"/>
+      <c r="E252" s="83"/>
+      <c r="F252" s="83"/>
+      <c r="G252" s="83"/>
+      <c r="H252" s="84"/>
     </row>
     <row r="253" spans="1:9" s="71" customFormat="1" ht="132" x14ac:dyDescent="0.3">
       <c r="A253" s="71" t="s">
@@ -21875,15 +21875,15 @@
       </c>
     </row>
     <row r="256" spans="1:9" s="71" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B256" s="86" t="s">
+      <c r="B256" s="82" t="s">
         <v>919</v>
       </c>
-      <c r="C256" s="87"/>
-      <c r="D256" s="87"/>
-      <c r="E256" s="87"/>
-      <c r="F256" s="87"/>
-      <c r="G256" s="87"/>
-      <c r="H256" s="88"/>
+      <c r="C256" s="83"/>
+      <c r="D256" s="83"/>
+      <c r="E256" s="83"/>
+      <c r="F256" s="83"/>
+      <c r="G256" s="83"/>
+      <c r="H256" s="84"/>
     </row>
     <row r="257" spans="1:9" s="71" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A257" s="71" t="s">
@@ -21915,15 +21915,15 @@
       </c>
     </row>
     <row r="258" spans="1:9" s="71" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B258" s="86" t="s">
+      <c r="B258" s="82" t="s">
         <v>923</v>
       </c>
-      <c r="C258" s="87"/>
-      <c r="D258" s="87"/>
-      <c r="E258" s="87"/>
-      <c r="F258" s="87"/>
-      <c r="G258" s="87"/>
-      <c r="H258" s="88"/>
+      <c r="C258" s="83"/>
+      <c r="D258" s="83"/>
+      <c r="E258" s="83"/>
+      <c r="F258" s="83"/>
+      <c r="G258" s="83"/>
+      <c r="H258" s="84"/>
     </row>
     <row r="259" spans="1:9" s="71" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A259" s="71" t="s">
@@ -22011,26 +22011,26 @@
       <c r="I261" s="74"/>
     </row>
     <row r="262" spans="1:9" s="71" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B262" s="86" t="s">
+      <c r="B262" s="82" t="s">
         <v>934</v>
       </c>
-      <c r="C262" s="87"/>
-      <c r="D262" s="87"/>
-      <c r="E262" s="87"/>
-      <c r="F262" s="87"/>
-      <c r="G262" s="87"/>
-      <c r="H262" s="88"/>
+      <c r="C262" s="83"/>
+      <c r="D262" s="83"/>
+      <c r="E262" s="83"/>
+      <c r="F262" s="83"/>
+      <c r="G262" s="83"/>
+      <c r="H262" s="84"/>
     </row>
     <row r="263" spans="1:9" s="71" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B263" s="89" t="s">
+      <c r="B263" s="85" t="s">
         <v>935</v>
       </c>
-      <c r="C263" s="90"/>
-      <c r="D263" s="90"/>
-      <c r="E263" s="90"/>
-      <c r="F263" s="90"/>
-      <c r="G263" s="90"/>
-      <c r="H263" s="91"/>
+      <c r="C263" s="86"/>
+      <c r="D263" s="86"/>
+      <c r="E263" s="86"/>
+      <c r="F263" s="86"/>
+      <c r="G263" s="86"/>
+      <c r="H263" s="87"/>
     </row>
     <row r="264" spans="1:9" s="71" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A264" s="71" t="s">
@@ -22116,15 +22116,15 @@
       </c>
     </row>
     <row r="267" spans="1:9" s="71" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B267" s="89" t="s">
+      <c r="B267" s="85" t="s">
         <v>947</v>
       </c>
-      <c r="C267" s="90"/>
-      <c r="D267" s="90"/>
-      <c r="E267" s="90"/>
-      <c r="F267" s="90"/>
-      <c r="G267" s="90"/>
-      <c r="H267" s="91"/>
+      <c r="C267" s="86"/>
+      <c r="D267" s="86"/>
+      <c r="E267" s="86"/>
+      <c r="F267" s="86"/>
+      <c r="G267" s="86"/>
+      <c r="H267" s="87"/>
     </row>
     <row r="268" spans="1:9" s="71" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A268" s="71" t="s">
@@ -22183,15 +22183,15 @@
       </c>
     </row>
     <row r="270" spans="1:9" s="71" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B270" s="89" t="s">
+      <c r="B270" s="85" t="s">
         <v>955</v>
       </c>
-      <c r="C270" s="90"/>
-      <c r="D270" s="90"/>
-      <c r="E270" s="90"/>
-      <c r="F270" s="90"/>
-      <c r="G270" s="90"/>
-      <c r="H270" s="91"/>
+      <c r="C270" s="86"/>
+      <c r="D270" s="86"/>
+      <c r="E270" s="86"/>
+      <c r="F270" s="86"/>
+      <c r="G270" s="86"/>
+      <c r="H270" s="87"/>
     </row>
     <row r="271" spans="1:9" s="71" customFormat="1" ht="132" x14ac:dyDescent="0.3">
       <c r="A271" s="71" t="s">
@@ -22329,52 +22329,70 @@
       </c>
     </row>
     <row r="276" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B276" s="92" t="s">
+      <c r="B276" s="88" t="s">
         <v>972</v>
       </c>
-      <c r="C276" s="92"/>
-      <c r="D276" s="92"/>
-      <c r="E276" s="92"/>
-      <c r="F276" s="92"/>
-      <c r="G276" s="92"/>
-      <c r="H276" s="92"/>
+      <c r="C276" s="88"/>
+      <c r="D276" s="88"/>
+      <c r="E276" s="88"/>
+      <c r="F276" s="88"/>
+      <c r="G276" s="88"/>
+      <c r="H276" s="88"/>
     </row>
     <row r="277" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B277" s="93" t="s">
+      <c r="B277" s="89" t="s">
         <v>973</v>
       </c>
-      <c r="C277" s="93"/>
-      <c r="D277" s="93"/>
-      <c r="E277" s="93"/>
-      <c r="F277" s="93"/>
-      <c r="G277" s="93"/>
-      <c r="H277" s="93"/>
+      <c r="C277" s="89"/>
+      <c r="D277" s="89"/>
+      <c r="E277" s="89"/>
+      <c r="F277" s="89"/>
+      <c r="G277" s="89"/>
+      <c r="H277" s="89"/>
     </row>
     <row r="278" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B278" s="93" t="s">
+      <c r="B278" s="89" t="s">
         <v>974</v>
       </c>
-      <c r="C278" s="93"/>
-      <c r="D278" s="93"/>
-      <c r="E278" s="93"/>
-      <c r="F278" s="93"/>
-      <c r="G278" s="93"/>
-      <c r="H278" s="93"/>
+      <c r="C278" s="89"/>
+      <c r="D278" s="89"/>
+      <c r="E278" s="89"/>
+      <c r="F278" s="89"/>
+      <c r="G278" s="89"/>
+      <c r="H278" s="89"/>
     </row>
     <row r="279" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B279" s="85" t="s">
+      <c r="B279" s="81" t="s">
         <v>975</v>
       </c>
-      <c r="C279" s="85"/>
-      <c r="D279" s="85"/>
-      <c r="E279" s="85"/>
-      <c r="F279" s="85"/>
-      <c r="G279" s="85"/>
-      <c r="H279" s="85"/>
+      <c r="C279" s="81"/>
+      <c r="D279" s="81"/>
+      <c r="E279" s="81"/>
+      <c r="F279" s="81"/>
+      <c r="G279" s="81"/>
+      <c r="H279" s="81"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:I279" xr:uid="{6B1B4B68-CDE7-4773-B6E3-1B4E74E676EC}"/>
   <mergeCells count="30">
+    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B243:H243"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="B101:H101"/>
+    <mergeCell ref="B108:H108"/>
+    <mergeCell ref="B125:H125"/>
+    <mergeCell ref="B138:H138"/>
+    <mergeCell ref="B153:H153"/>
+    <mergeCell ref="B169:H169"/>
+    <mergeCell ref="B183:H183"/>
+    <mergeCell ref="B192:H192"/>
+    <mergeCell ref="B203:H203"/>
+    <mergeCell ref="B218:H218"/>
     <mergeCell ref="B279:H279"/>
     <mergeCell ref="B244:H244"/>
     <mergeCell ref="B252:H252"/>
@@ -22387,24 +22405,6 @@
     <mergeCell ref="B276:H276"/>
     <mergeCell ref="B277:H277"/>
     <mergeCell ref="B278:H278"/>
-    <mergeCell ref="B243:H243"/>
-    <mergeCell ref="B89:H89"/>
-    <mergeCell ref="B101:H101"/>
-    <mergeCell ref="B108:H108"/>
-    <mergeCell ref="B125:H125"/>
-    <mergeCell ref="B138:H138"/>
-    <mergeCell ref="B153:H153"/>
-    <mergeCell ref="B169:H169"/>
-    <mergeCell ref="B183:H183"/>
-    <mergeCell ref="B192:H192"/>
-    <mergeCell ref="B203:H203"/>
-    <mergeCell ref="B218:H218"/>
-    <mergeCell ref="B74:H74"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B61:H61"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
   <pageSetup scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -22423,7 +22423,7 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -22442,14 +22442,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="93" t="s">
         <v>1047</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
     </row>
     <row r="2" spans="1:13" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
@@ -22631,9 +22631,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22860,19 +22863,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB365EA7-6D7C-4914-BFB9-6D46B124F572}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0E031C4-B4FD-4645-82D1-7F57E6C194D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22897,9 +22896,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0E031C4-B4FD-4645-82D1-7F57E6C194D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB365EA7-6D7C-4914-BFB9-6D46B124F572}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>